<commit_message>
cap nhat noi dung 221018
</commit_message>
<xml_diff>
--- a/Eil/03.Bảng giá-220616.xlsx
+++ b/Eil/03.Bảng giá-220616.xlsx
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Thống kê'!$B$5:$C$5</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="0">'Thống kê'!$H$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">'Thống kê'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Giá Gốc'!$A$1:$K$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Giá Gốc'!$A$1:$L$60</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -442,9 +442,6 @@
     <t>Tùy chỉnh</t>
   </si>
   <si>
-    <t>CHÍNH SÁCH GIÁ NHÀ PHÂN PHỐI - ÁP DỤNG TỪ THÁNG 08/2022</t>
-  </si>
-  <si>
     <t>PP Bag</t>
   </si>
   <si>
@@ -661,9 +658,6 @@
     <t>23*30</t>
   </si>
   <si>
-    <t>Listed price</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -755,6 +749,12 @@
   </si>
   <si>
     <t>VND</t>
+  </si>
+  <si>
+    <t>Price (Kg)</t>
+  </si>
+  <si>
+    <t>CHÍNH SÁCH GIÁ ĐẠI LÝ</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1067,20 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1080,10 +1090,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1091,10 +1104,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1111,16 +1121,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1460,36 +1460,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
+      <c r="A1" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="5" spans="1:13" s="15" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
@@ -2528,19 +2528,19 @@
         <v>96</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>97</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O5" s="14" t="s">
         <v>95</v>
@@ -2562,7 +2562,7 @@
         <v>TM</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F6" s="3" t="str">
         <f>IFERROR(VLOOKUP(E6,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2617,7 +2617,7 @@
         <v>TM</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="3" t="str">
         <f>IFERROR(VLOOKUP(E7,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2672,7 +2672,7 @@
         <v>TM</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8" s="3" t="str">
         <f>IFERROR(VLOOKUP(E8,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2720,14 +2720,14 @@
         <v>44780</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="3" t="str">
         <f>IFERROR(VLOOKUP(E9,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2775,7 +2775,7 @@
         <v>44780</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2830,14 +2830,14 @@
         <v>44780</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F11" s="3" t="str">
         <f>IFERROR(VLOOKUP(E11,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2885,14 +2885,14 @@
         <v>44780</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="3" t="str">
         <f>IFERROR(VLOOKUP(E12,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2940,14 +2940,14 @@
         <v>44780</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F13" s="3" t="str">
         <f>IFERROR(VLOOKUP(E13,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -2995,14 +2995,14 @@
         <v>44780</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F14" s="3" t="str">
         <f>IFERROR(VLOOKUP(E14,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3050,14 +3050,14 @@
         <v>44780</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F15" s="3" t="str">
         <f>IFERROR(VLOOKUP(E15,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3105,7 +3105,7 @@
         <v>44780</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3160,14 +3160,14 @@
         <v>44780</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F17" s="3" t="str">
         <f>IFERROR(VLOOKUP(E17,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3215,14 +3215,14 @@
         <v>44780</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F18" s="3" t="str">
         <f>IFERROR(VLOOKUP(E18,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3270,14 +3270,14 @@
         <v>44780</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TM</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F19" s="3" t="str">
         <f>IFERROR(VLOOKUP(E19,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3325,14 +3325,14 @@
         <v>44780</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>SX</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F20" s="3" t="str">
         <f>IFERROR(VLOOKUP(E20,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3380,14 +3380,14 @@
         <v>44780</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>SX</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F21" s="3" t="str">
         <f>IFERROR(VLOOKUP(E21,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3435,7 +3435,7 @@
         <v>44780</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3490,14 +3490,14 @@
         <v>44780</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>SX</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F23" s="3" t="str">
         <f>IFERROR(VLOOKUP(E23,'Giá Gốc'!$B$7:$P$98,2,0),"")</f>
@@ -3569,10 +3569,8 @@
   </sheetPr>
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,28 +3586,30 @@
     <col min="10" max="10" width="8.5546875" style="34" customWidth="1"/>
     <col min="11" max="11" width="8.44140625" style="36" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="10" hidden="1" customWidth="1"/>
     <col min="15" max="16" width="8" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="5.44140625" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="14.77734375" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="0" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5546875" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="A1" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
@@ -3625,131 +3625,131 @@
       <c r="K2" s="26"/>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="58" t="s">
+      <c r="A4" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="E4" s="58" t="s">
-        <v>190</v>
-      </c>
-      <c r="F4" s="58" t="s">
+      <c r="G4" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="I4" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="H4" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="I4" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="58" t="s">
-        <v>211</v>
-      </c>
-      <c r="M4" s="63" t="s">
-        <v>209</v>
-      </c>
-      <c r="N4" s="65" t="s">
+      <c r="L4" s="61" t="s">
+        <v>241</v>
+      </c>
+      <c r="M4" s="67" t="s">
+        <v>208</v>
+      </c>
+      <c r="N4" s="69" t="s">
+        <v>236</v>
+      </c>
+      <c r="O4" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="P4" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q4" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="R4" s="63" t="s">
+        <v>234</v>
+      </c>
+      <c r="S4" s="66" t="s">
+        <v>237</v>
+      </c>
+      <c r="T4" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="O4" s="58" t="s">
-        <v>212</v>
-      </c>
-      <c r="P4" s="58" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q4" s="58" t="s">
-        <v>235</v>
-      </c>
-      <c r="R4" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="S4" s="54" t="s">
+      <c r="U4" s="66" t="s">
         <v>239</v>
       </c>
-      <c r="T4" s="54" t="s">
+      <c r="V4" s="66"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="U4" s="54" t="s">
-        <v>241</v>
-      </c>
-      <c r="V4" s="54"/>
-      <c r="W4" s="69"/>
-      <c r="X4" s="2" t="s">
-        <v>242</v>
-      </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="54"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="71">
+      <c r="A5" s="63"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="55">
         <v>23500</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="68"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="62"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>59</v>
@@ -3769,7 +3769,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I7" s="28">
         <v>1</v>
@@ -3803,8 +3803,8 @@
         <f>N7/O7-100%</f>
         <v>0.25090909090909097</v>
       </c>
-      <c r="R7" s="67" t="s">
-        <v>237</v>
+      <c r="R7" s="71" t="s">
+        <v>235</v>
       </c>
       <c r="S7" s="18">
         <f>$M7*0.95</f>
@@ -3823,15 +3823,15 @@
         <v>-1000</v>
       </c>
       <c r="W7" s="18"/>
-      <c r="X7" s="70">
+      <c r="X7" s="54">
         <f>ROUND(S7/$X$5,2)</f>
         <v>1.26</v>
       </c>
-      <c r="Y7" s="70">
+      <c r="Y7" s="54">
         <f t="shared" ref="Y7:Z7" si="4">ROUND(T7/$X$5,2)</f>
         <v>1.19</v>
       </c>
-      <c r="Z7" s="70">
+      <c r="Z7" s="54">
         <f t="shared" si="4"/>
         <v>1.1299999999999999</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>60</v>
@@ -3861,7 +3861,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I8" s="28">
         <v>1</v>
@@ -3895,7 +3895,7 @@
         <f t="shared" ref="Q8:Q60" si="6">N8/O8-100%</f>
         <v>0.469090909090909</v>
       </c>
-      <c r="R8" s="67"/>
+      <c r="R8" s="71"/>
       <c r="S8" s="18">
         <f t="shared" ref="S8:S60" si="7">$M8*0.95</f>
         <v>37240</v>
@@ -3913,15 +3913,15 @@
         <v>1000</v>
       </c>
       <c r="W8" s="18"/>
-      <c r="X8" s="70">
+      <c r="X8" s="54">
         <f t="shared" ref="X8:X11" si="11">ROUND(S8/$X$5,2)</f>
         <v>1.58</v>
       </c>
-      <c r="Y8" s="70">
+      <c r="Y8" s="54">
         <f t="shared" ref="Y8:Y11" si="12">ROUND(T8/$X$5,2)</f>
         <v>1.5</v>
       </c>
-      <c r="Z8" s="70">
+      <c r="Z8" s="54">
         <f t="shared" ref="Z8:Z11" si="13">ROUND(U8/$X$5,2)</f>
         <v>1.42</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>61</v>
@@ -3951,7 +3951,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I9" s="28">
         <v>1</v>
@@ -3985,7 +3985,7 @@
         <f t="shared" si="6"/>
         <v>0.44727272727272727</v>
       </c>
-      <c r="R9" s="67"/>
+      <c r="R9" s="71"/>
       <c r="S9" s="18">
         <f t="shared" si="7"/>
         <v>36480</v>
@@ -4003,15 +4003,15 @@
         <v>800</v>
       </c>
       <c r="W9" s="18"/>
-      <c r="X9" s="70">
+      <c r="X9" s="54">
         <f t="shared" si="11"/>
         <v>1.55</v>
       </c>
-      <c r="Y9" s="70">
+      <c r="Y9" s="54">
         <f t="shared" si="12"/>
         <v>1.47</v>
       </c>
-      <c r="Z9" s="70">
+      <c r="Z9" s="54">
         <f t="shared" si="13"/>
         <v>1.39</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>62</v>
@@ -4041,7 +4041,7 @@
         <v>16</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I10" s="28">
         <v>1</v>
@@ -4075,7 +4075,7 @@
         <f t="shared" si="6"/>
         <v>0.42545454545454553</v>
       </c>
-      <c r="R10" s="67"/>
+      <c r="R10" s="71"/>
       <c r="S10" s="18">
         <f t="shared" si="7"/>
         <v>35720</v>
@@ -4093,15 +4093,15 @@
         <v>600</v>
       </c>
       <c r="W10" s="18"/>
-      <c r="X10" s="70">
+      <c r="X10" s="54">
         <f t="shared" si="11"/>
         <v>1.52</v>
       </c>
-      <c r="Y10" s="70">
+      <c r="Y10" s="54">
         <f t="shared" si="12"/>
         <v>1.44</v>
       </c>
-      <c r="Z10" s="70">
+      <c r="Z10" s="54">
         <f t="shared" si="13"/>
         <v>1.36</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>63</v>
@@ -4131,7 +4131,7 @@
         <v>18</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I11" s="28">
         <v>1</v>
@@ -4165,7 +4165,7 @@
         <f t="shared" si="6"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="R11" s="67"/>
+      <c r="R11" s="71"/>
       <c r="S11" s="18">
         <f t="shared" si="7"/>
         <v>30400</v>
@@ -4183,15 +4183,15 @@
         <v>-800</v>
       </c>
       <c r="W11" s="18"/>
-      <c r="X11" s="70">
+      <c r="X11" s="54">
         <f t="shared" si="11"/>
         <v>1.29</v>
       </c>
-      <c r="Y11" s="70">
+      <c r="Y11" s="54">
         <f t="shared" si="12"/>
         <v>1.23</v>
       </c>
-      <c r="Z11" s="70">
+      <c r="Z11" s="54">
         <f t="shared" si="13"/>
         <v>1.1599999999999999</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>64</v>
@@ -4222,7 +4222,7 @@
         <v>24</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I12" s="28">
         <f>1000/E12*2</f>
@@ -4257,7 +4257,7 @@
         <f t="shared" si="6"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="R12" s="67"/>
+      <c r="R12" s="71"/>
       <c r="S12" s="18">
         <f t="shared" si="7"/>
         <v>30400</v>
@@ -4281,7 +4281,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>65</v>
@@ -4302,7 +4302,7 @@
         <v>60</v>
       </c>
       <c r="H13" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I13" s="28">
         <f>1000/E13*2.5</f>
@@ -4337,7 +4337,7 @@
         <f t="shared" si="6"/>
         <v>0.29454545454545444</v>
       </c>
-      <c r="R13" s="67"/>
+      <c r="R13" s="71"/>
       <c r="S13" s="18">
         <f t="shared" si="7"/>
         <v>31160</v>
@@ -4361,7 +4361,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>66</v>
@@ -4382,7 +4382,7 @@
         <v>60</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I14" s="28">
         <f>1000/E14*2</f>
@@ -4417,7 +4417,7 @@
         <f t="shared" si="6"/>
         <v>0.3163636363636364</v>
       </c>
-      <c r="R14" s="67"/>
+      <c r="R14" s="71"/>
       <c r="S14" s="18">
         <f t="shared" si="7"/>
         <v>31920</v>
@@ -4441,7 +4441,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>67</v>
@@ -4462,7 +4462,7 @@
         <v>100</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I15" s="28">
         <f t="shared" ref="I15:I21" si="17">1000/E15*2.5</f>
@@ -4497,7 +4497,7 @@
         <f t="shared" si="6"/>
         <v>0.3600000000000001</v>
       </c>
-      <c r="R15" s="67"/>
+      <c r="R15" s="71"/>
       <c r="S15" s="18">
         <f t="shared" si="7"/>
         <v>33440</v>
@@ -4521,7 +4521,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>68</v>
@@ -4542,7 +4542,7 @@
         <v>200</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I16" s="28">
         <f t="shared" si="17"/>
@@ -4577,7 +4577,7 @@
         <f t="shared" si="6"/>
         <v>0.40363636363636357</v>
       </c>
-      <c r="R16" s="67"/>
+      <c r="R16" s="71"/>
       <c r="S16" s="18">
         <f t="shared" si="7"/>
         <v>34960</v>
@@ -4601,7 +4601,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>69</v>
@@ -4622,7 +4622,7 @@
         <v>400</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I17" s="28">
         <f t="shared" si="17"/>
@@ -4657,7 +4657,7 @@
         <f t="shared" si="6"/>
         <v>0.469090909090909</v>
       </c>
-      <c r="R17" s="67"/>
+      <c r="R17" s="71"/>
       <c r="S17" s="18">
         <f t="shared" si="7"/>
         <v>37240</v>
@@ -4681,7 +4681,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>70</v>
@@ -4702,7 +4702,7 @@
         <v>500</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I18" s="28">
         <f t="shared" si="17"/>
@@ -4737,7 +4737,7 @@
         <f>N18/O18-100%</f>
         <v>0.49090909090909096</v>
       </c>
-      <c r="R18" s="67"/>
+      <c r="R18" s="71"/>
       <c r="S18" s="18">
         <f t="shared" si="7"/>
         <v>38000</v>
@@ -4782,7 +4782,7 @@
         <v>1000</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I19" s="28">
         <f t="shared" si="17"/>
@@ -4817,7 +4817,7 @@
         <f t="shared" si="6"/>
         <v>0.57818181818181813</v>
       </c>
-      <c r="R19" s="67"/>
+      <c r="R19" s="71"/>
       <c r="S19" s="18">
         <f t="shared" si="7"/>
         <v>41040</v>
@@ -4841,7 +4841,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>72</v>
@@ -4862,7 +4862,7 @@
         <v>2000</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I20" s="28">
         <f t="shared" si="17"/>
@@ -4897,7 +4897,7 @@
         <f>N20/O20-100%</f>
         <v>0.88363636363636355</v>
       </c>
-      <c r="R20" s="67"/>
+      <c r="R20" s="71"/>
       <c r="S20" s="18">
         <f t="shared" si="7"/>
         <v>51680</v>
@@ -4921,7 +4921,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>107</v>
@@ -4942,7 +4942,7 @@
         <v>5000</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I21" s="28">
         <f t="shared" si="17"/>
@@ -4977,7 +4977,7 @@
         <f t="shared" si="6"/>
         <v>1.8872727272727272</v>
       </c>
-      <c r="R21" s="67"/>
+      <c r="R21" s="71"/>
       <c r="S21" s="18">
         <f t="shared" si="7"/>
         <v>86640</v>
@@ -4996,20 +4996,20 @@
       </c>
       <c r="W21" s="18"/>
     </row>
-    <row r="22" spans="1:23" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="62" t="s">
+    <row r="22" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
       <c r="N22" s="46"/>
@@ -5035,12 +5035,12 @@
       </c>
       <c r="W22" s="18"/>
     </row>
-    <row r="23" spans="1:23" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>48</v>
@@ -5060,7 +5060,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I23" s="28">
         <v>1</v>
@@ -5070,7 +5070,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L23" s="19">
         <v>22000</v>
@@ -5114,12 +5114,12 @@
       </c>
       <c r="W23" s="18"/>
     </row>
-    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>109</v>
@@ -5139,7 +5139,7 @@
         <v>10</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I24" s="28">
         <v>1</v>
@@ -5149,7 +5149,7 @@
         <v>10</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L24" s="19">
         <v>22000</v>
@@ -5193,12 +5193,12 @@
       </c>
       <c r="W24" s="18"/>
     </row>
-    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>49</v>
@@ -5218,7 +5218,7 @@
         <v>25</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I25" s="28">
         <v>1</v>
@@ -5228,7 +5228,7 @@
         <v>25</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L25" s="19">
         <v>20000</v>
@@ -5272,12 +5272,12 @@
       </c>
       <c r="W25" s="18"/>
     </row>
-    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>50</v>
@@ -5297,7 +5297,7 @@
         <v>50</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="31">
@@ -5305,7 +5305,7 @@
         <v>25</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L26" s="19">
         <v>22000</v>
@@ -5349,12 +5349,12 @@
       </c>
       <c r="W26" s="18"/>
     </row>
-    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>5</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>51</v>
@@ -5374,7 +5374,7 @@
         <v>120</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="31">
@@ -5382,7 +5382,7 @@
         <v>24</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L27" s="19">
         <v>22000</v>
@@ -5426,12 +5426,12 @@
       </c>
       <c r="W27" s="18"/>
     </row>
-    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>52</v>
@@ -5452,7 +5452,7 @@
         <v>240</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I28" s="28">
         <f>1000/E28*8</f>
@@ -5463,7 +5463,7 @@
         <v>24</v>
       </c>
       <c r="K28" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L28" s="19">
         <v>22000</v>
@@ -5507,12 +5507,12 @@
       </c>
       <c r="W28" s="18"/>
     </row>
-    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>53</v>
@@ -5533,7 +5533,7 @@
         <v>480</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I29" s="28">
         <f>1000/E29*8</f>
@@ -5544,7 +5544,7 @@
         <v>24</v>
       </c>
       <c r="K29" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L29" s="19">
         <v>22000</v>
@@ -5588,12 +5588,12 @@
       </c>
       <c r="W29" s="18"/>
     </row>
-    <row r="30" spans="1:23" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>8</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>54</v>
@@ -5614,7 +5614,7 @@
         <v>1200</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I30" s="28">
         <f>1000/E30*8</f>
@@ -5625,7 +5625,7 @@
         <v>24</v>
       </c>
       <c r="K30" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L30" s="19">
         <v>22000</v>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="W30" s="18"/>
     </row>
-    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>9</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>2100</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I31" s="28">
         <f>1000/E31*7</f>
@@ -5706,7 +5706,7 @@
         <v>21</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L31" s="19">
         <v>24000</v>
@@ -5750,12 +5750,12 @@
       </c>
       <c r="W31" s="18"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>56</v>
@@ -5776,7 +5776,7 @@
         <v>3600</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I32" s="28">
         <f>1000/E32*6</f>
@@ -5787,7 +5787,7 @@
         <v>18</v>
       </c>
       <c r="K32" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L32" s="19">
         <v>24000</v>
@@ -5831,12 +5831,12 @@
       </c>
       <c r="W32" s="18"/>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>57</v>
@@ -5857,7 +5857,7 @@
         <v>6000</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I33" s="28">
         <f>1000/E33*6</f>
@@ -5868,7 +5868,7 @@
         <v>18</v>
       </c>
       <c r="K33" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L33" s="19">
         <v>35000</v>
@@ -5912,12 +5912,12 @@
       </c>
       <c r="W33" s="18"/>
     </row>
-    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>12</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>58</v>
@@ -5938,7 +5938,7 @@
         <v>9000</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I34" s="28">
         <f>1000/E34*6</f>
@@ -5949,7 +5949,7 @@
         <v>18</v>
       </c>
       <c r="K34" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L34" s="19">
         <v>35000</v>
@@ -5993,15 +5993,15 @@
       </c>
       <c r="W34" s="18"/>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D35" s="42" t="str">
         <f t="shared" ref="D35" si="27">RIGHT(C35,LEN(C35)-5)</f>
@@ -6019,7 +6019,7 @@
         <v>14286</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I35" s="28">
         <f>1000/E35*5</f>
@@ -6030,7 +6030,7 @@
         <v>20.000399999999999</v>
       </c>
       <c r="K35" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L35" s="19">
         <v>35000</v>
@@ -6074,20 +6074,20 @@
       </c>
       <c r="W35" s="18"/>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="62" t="s">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A36" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="62"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
       <c r="L36" s="39"/>
       <c r="M36" s="39"/>
       <c r="N36" s="17"/>
@@ -6113,12 +6113,12 @@
       </c>
       <c r="W36" s="18"/>
     </row>
-    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>1</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>11</v>
@@ -6138,7 +6138,7 @@
         <v>18</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I37" s="28">
         <v>1</v>
@@ -6148,7 +6148,7 @@
         <v>18</v>
       </c>
       <c r="K37" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L37" s="19">
         <v>44000</v>
@@ -6192,12 +6192,12 @@
       </c>
       <c r="W37" s="18"/>
     </row>
-    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>10</v>
@@ -6217,7 +6217,7 @@
         <v>16</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I38" s="28">
         <v>1</v>
@@ -6227,7 +6227,7 @@
         <v>16</v>
       </c>
       <c r="K38" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L38" s="19">
         <v>44000</v>
@@ -6271,12 +6271,12 @@
       </c>
       <c r="W38" s="18"/>
     </row>
-    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>108</v>
@@ -6296,7 +6296,7 @@
         <v>18</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I39" s="28">
         <v>1</v>
@@ -6306,7 +6306,7 @@
         <v>18</v>
       </c>
       <c r="K39" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L39" s="19">
         <v>42000</v>
@@ -6350,12 +6350,12 @@
       </c>
       <c r="W39" s="18"/>
     </row>
-    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>4</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>12</v>
@@ -6375,7 +6375,7 @@
         <v>40</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I40" s="32"/>
       <c r="J40" s="31">
@@ -6383,7 +6383,7 @@
         <v>20</v>
       </c>
       <c r="K40" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L40" s="19">
         <v>44000</v>
@@ -6427,12 +6427,12 @@
       </c>
       <c r="W40" s="18"/>
     </row>
-    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>5</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>13</v>
@@ -6452,7 +6452,7 @@
         <v>120</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I41" s="32"/>
       <c r="J41" s="31">
@@ -6460,7 +6460,7 @@
         <v>24</v>
       </c>
       <c r="K41" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L41" s="19">
         <v>44000</v>
@@ -6504,12 +6504,12 @@
       </c>
       <c r="W41" s="18"/>
     </row>
-    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>6</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>14</v>
@@ -6530,7 +6530,7 @@
         <v>300</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I42" s="28">
         <f t="shared" ref="I42:I49" si="35">1000/E42*2.5</f>
@@ -6541,7 +6541,7 @@
         <v>30</v>
       </c>
       <c r="K42" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L42" s="19">
         <v>44000</v>
@@ -6585,12 +6585,12 @@
       </c>
       <c r="W42" s="18"/>
     </row>
-    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>7</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>15</v>
@@ -6611,7 +6611,7 @@
         <v>600</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I43" s="28">
         <f t="shared" si="35"/>
@@ -6622,7 +6622,7 @@
         <v>30</v>
       </c>
       <c r="K43" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L43" s="19">
         <v>44000</v>
@@ -6666,12 +6666,12 @@
       </c>
       <c r="W43" s="18"/>
     </row>
-    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>8</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>17</v>
@@ -6692,7 +6692,7 @@
         <v>1200</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I44" s="28">
         <f t="shared" si="35"/>
@@ -6703,7 +6703,7 @@
         <v>30</v>
       </c>
       <c r="K44" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L44" s="19">
         <v>44000</v>
@@ -6747,12 +6747,12 @@
       </c>
       <c r="W44" s="18"/>
     </row>
-    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>18</v>
@@ -6773,7 +6773,7 @@
         <v>1500</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I45" s="28">
         <f t="shared" si="35"/>
@@ -6784,7 +6784,7 @@
         <v>30</v>
       </c>
       <c r="K45" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L45" s="19">
         <v>44000</v>
@@ -6828,7 +6828,7 @@
       </c>
       <c r="W45" s="18"/>
     </row>
-    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>10</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>3000</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I46" s="28">
         <f t="shared" si="35"/>
@@ -6865,7 +6865,7 @@
         <v>30</v>
       </c>
       <c r="K46" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L46" s="19">
         <v>46000</v>
@@ -6909,12 +6909,12 @@
       </c>
       <c r="W46" s="18"/>
     </row>
-    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>11</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>20</v>
@@ -6935,7 +6935,7 @@
         <v>5000</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I47" s="28">
         <f t="shared" si="35"/>
@@ -6946,7 +6946,7 @@
         <v>25</v>
       </c>
       <c r="K47" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L47" s="19">
         <v>46000</v>
@@ -6990,12 +6990,12 @@
       </c>
       <c r="W47" s="18"/>
     </row>
-    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>12</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>21</v>
@@ -7016,7 +7016,7 @@
         <v>8334</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I48" s="28">
         <f t="shared" si="35"/>
@@ -7027,7 +7027,7 @@
         <v>25.001999999999999</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L48" s="19">
         <v>50000</v>
@@ -7071,12 +7071,12 @@
       </c>
       <c r="W48" s="18"/>
     </row>
-    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>13</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>22</v>
@@ -7097,7 +7097,7 @@
         <v>12500</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I49" s="28">
         <f t="shared" si="35"/>
@@ -7108,7 +7108,7 @@
         <v>25</v>
       </c>
       <c r="K49" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L49" s="19">
         <v>50000</v>
@@ -7152,15 +7152,15 @@
       </c>
       <c r="W49" s="18"/>
     </row>
-    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>14</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D50" s="42" t="str">
         <f t="shared" si="29"/>
@@ -7178,7 +7178,7 @@
         <v>8334</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I50" s="28">
         <f>1000/E50</f>
@@ -7189,7 +7189,7 @@
         <v>10.0008</v>
       </c>
       <c r="K50" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L50" s="19">
         <v>50000</v>
@@ -7234,26 +7234,26 @@
       <c r="W50" s="18"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A51" s="55" t="s">
+      <c r="A51" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="56"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="56"/>
-      <c r="K51" s="56"/>
-      <c r="L51" s="56"/>
-      <c r="M51" s="56"/>
-      <c r="N51" s="56"/>
-      <c r="O51" s="56"/>
-      <c r="P51" s="56"/>
-      <c r="Q51" s="56"/>
-      <c r="R51" s="68"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="60"/>
+      <c r="L51" s="60"/>
+      <c r="M51" s="60"/>
+      <c r="N51" s="60"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="60"/>
+      <c r="Q51" s="60"/>
+      <c r="R51" s="62"/>
       <c r="S51" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -7277,13 +7277,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E52" s="4">
         <v>1.5</v>
@@ -7295,7 +7295,7 @@
         <v>7200</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I52" s="28">
         <v>667</v>
@@ -7329,8 +7329,8 @@
         <f t="shared" si="6"/>
         <v>2.0181818181818181</v>
       </c>
-      <c r="R52" s="67" t="s">
-        <v>237</v>
+      <c r="R52" s="71" t="s">
+        <v>235</v>
       </c>
       <c r="S52" s="18">
         <f t="shared" si="7"/>
@@ -7355,13 +7355,13 @@
         <v>2</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E53" s="4">
         <v>2</v>
@@ -7373,7 +7373,7 @@
         <v>4800</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I53" s="28">
         <v>500</v>
@@ -7407,7 +7407,7 @@
         <f t="shared" si="6"/>
         <v>1.7563636363636363</v>
       </c>
-      <c r="R53" s="67"/>
+      <c r="R53" s="71"/>
       <c r="S53" s="18">
         <f t="shared" si="7"/>
         <v>82080</v>
@@ -7431,13 +7431,13 @@
         <v>3</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E54" s="4">
         <v>4</v>
@@ -7449,7 +7449,7 @@
         <v>2400</v>
       </c>
       <c r="H54" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I54" s="28">
         <v>250</v>
@@ -7483,7 +7483,7 @@
         <f t="shared" si="6"/>
         <v>0.77454545454545465</v>
       </c>
-      <c r="R54" s="67"/>
+      <c r="R54" s="71"/>
       <c r="S54" s="18">
         <f t="shared" si="7"/>
         <v>47880</v>
@@ -7507,13 +7507,13 @@
         <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E55" s="4">
         <v>8</v>
@@ -7525,7 +7525,7 @@
         <v>2400</v>
       </c>
       <c r="H55" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I55" s="28">
         <v>150</v>
@@ -7559,7 +7559,7 @@
         <f t="shared" si="6"/>
         <v>0.3600000000000001</v>
       </c>
-      <c r="R55" s="67"/>
+      <c r="R55" s="71"/>
       <c r="S55" s="18">
         <f t="shared" si="7"/>
         <v>33440</v>
@@ -7583,13 +7583,13 @@
         <v>5</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E56" s="4">
         <v>11</v>
@@ -7601,7 +7601,7 @@
         <v>1400</v>
       </c>
       <c r="H56" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I56" s="28">
         <v>120</v>
@@ -7635,7 +7635,7 @@
         <f t="shared" si="6"/>
         <v>0.33818181818181814</v>
       </c>
-      <c r="R56" s="67"/>
+      <c r="R56" s="71"/>
       <c r="S56" s="18">
         <f t="shared" si="7"/>
         <v>32680</v>
@@ -7659,13 +7659,13 @@
         <v>6</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E57" s="4">
         <v>17</v>
@@ -7677,7 +7677,7 @@
         <v>960</v>
       </c>
       <c r="H57" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I57" s="28">
         <v>60</v>
@@ -7711,7 +7711,7 @@
         <f t="shared" si="6"/>
         <v>0.14181818181818184</v>
       </c>
-      <c r="R57" s="67"/>
+      <c r="R57" s="71"/>
       <c r="S57" s="18">
         <f t="shared" si="7"/>
         <v>25840</v>
@@ -7731,26 +7731,26 @@
       <c r="W57" s="18"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="56"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
-      <c r="J58" s="56"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
-      <c r="O58" s="56"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="56"/>
-      <c r="R58" s="68"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="60"/>
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="60"/>
+      <c r="J58" s="60"/>
+      <c r="K58" s="60"/>
+      <c r="L58" s="60"/>
+      <c r="M58" s="60"/>
+      <c r="N58" s="60"/>
+      <c r="O58" s="60"/>
+      <c r="P58" s="60"/>
+      <c r="Q58" s="60"/>
+      <c r="R58" s="62"/>
       <c r="S58" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -7774,7 +7774,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>44</v>
@@ -7794,7 +7794,7 @@
         <v>2400</v>
       </c>
       <c r="H59" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I59" s="28">
         <v>200</v>
@@ -7828,8 +7828,8 @@
         <f t="shared" si="6"/>
         <v>0.19338842975206583</v>
       </c>
-      <c r="R59" s="67" t="s">
-        <v>237</v>
+      <c r="R59" s="71" t="s">
+        <v>235</v>
       </c>
       <c r="S59" s="18">
         <f t="shared" si="7"/>
@@ -7854,7 +7854,7 @@
         <v>2</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>45</v>
@@ -7874,7 +7874,7 @@
         <v>1500</v>
       </c>
       <c r="H60" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I60" s="28">
         <v>150</v>
@@ -7908,7 +7908,7 @@
         <f t="shared" si="6"/>
         <v>0.19338842975206583</v>
       </c>
-      <c r="R60" s="67"/>
+      <c r="R60" s="71"/>
       <c r="S60" s="18">
         <f t="shared" si="7"/>
         <v>30400</v>
@@ -7927,20 +7927,20 @@
       </c>
       <c r="W60" s="18"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A61" s="55" t="s">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B61" s="56"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
-      <c r="J61" s="56"/>
-      <c r="K61" s="56"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
       <c r="M61" s="18"/>
     </row>
     <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
@@ -8167,20 +8167,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="55" t="s">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B69" s="56"/>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="56"/>
-      <c r="J69" s="56"/>
-      <c r="K69" s="56"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="60"/>
+      <c r="D69" s="60"/>
+      <c r="E69" s="60"/>
+      <c r="F69" s="60"/>
+      <c r="G69" s="60"/>
+      <c r="H69" s="60"/>
+      <c r="I69" s="60"/>
+      <c r="J69" s="60"/>
+      <c r="K69" s="60"/>
     </row>
     <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
@@ -8243,20 +8243,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="55" t="s">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="56"/>
-      <c r="C72" s="56"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
-      <c r="G72" s="56"/>
-      <c r="H72" s="56"/>
-      <c r="I72" s="56"/>
-      <c r="J72" s="56"/>
-      <c r="K72" s="56"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="60"/>
+      <c r="J72" s="60"/>
+      <c r="K72" s="60"/>
     </row>
     <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
@@ -8310,20 +8310,20 @@
       <c r="J76" s="29"/>
       <c r="K76" s="30"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="55" t="s">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B77" s="56"/>
-      <c r="C77" s="56"/>
-      <c r="D77" s="56"/>
-      <c r="E77" s="56"/>
-      <c r="F77" s="56"/>
-      <c r="G77" s="56"/>
-      <c r="H77" s="56"/>
-      <c r="I77" s="56"/>
-      <c r="J77" s="56"/>
-      <c r="K77" s="56"/>
+      <c r="B77" s="60"/>
+      <c r="C77" s="60"/>
+      <c r="D77" s="60"/>
+      <c r="E77" s="60"/>
+      <c r="F77" s="60"/>
+      <c r="G77" s="60"/>
+      <c r="H77" s="60"/>
+      <c r="I77" s="60"/>
+      <c r="J77" s="60"/>
+      <c r="K77" s="60"/>
     </row>
     <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
@@ -8377,20 +8377,20 @@
       <c r="J81" s="29"/>
       <c r="K81" s="30"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A82" s="55" t="s">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B82" s="56"/>
-      <c r="C82" s="56"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
-      <c r="F82" s="56"/>
-      <c r="G82" s="56"/>
-      <c r="H82" s="56"/>
-      <c r="I82" s="56"/>
-      <c r="J82" s="56"/>
-      <c r="K82" s="56"/>
+      <c r="B82" s="60"/>
+      <c r="C82" s="60"/>
+      <c r="D82" s="60"/>
+      <c r="E82" s="60"/>
+      <c r="F82" s="60"/>
+      <c r="G82" s="60"/>
+      <c r="H82" s="60"/>
+      <c r="I82" s="60"/>
+      <c r="J82" s="60"/>
+      <c r="K82" s="60"/>
     </row>
     <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
@@ -8444,20 +8444,20 @@
       <c r="J86" s="29"/>
       <c r="K86" s="30"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A87" s="55" t="s">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B87" s="56"/>
-      <c r="C87" s="56"/>
-      <c r="D87" s="56"/>
-      <c r="E87" s="56"/>
-      <c r="F87" s="56"/>
-      <c r="G87" s="56"/>
-      <c r="H87" s="56"/>
-      <c r="I87" s="56"/>
-      <c r="J87" s="56"/>
-      <c r="K87" s="56"/>
+      <c r="B87" s="60"/>
+      <c r="C87" s="60"/>
+      <c r="D87" s="60"/>
+      <c r="E87" s="60"/>
+      <c r="F87" s="60"/>
+      <c r="G87" s="60"/>
+      <c r="H87" s="60"/>
+      <c r="I87" s="60"/>
+      <c r="J87" s="60"/>
+      <c r="K87" s="60"/>
     </row>
     <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
@@ -8511,20 +8511,20 @@
       <c r="J91" s="29"/>
       <c r="K91" s="30"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="55" t="s">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B92" s="56"/>
-      <c r="C92" s="56"/>
-      <c r="D92" s="56"/>
-      <c r="E92" s="56"/>
-      <c r="F92" s="56"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="56"/>
-      <c r="I92" s="56"/>
-      <c r="J92" s="56"/>
-      <c r="K92" s="56"/>
+      <c r="B92" s="60"/>
+      <c r="C92" s="60"/>
+      <c r="D92" s="60"/>
+      <c r="E92" s="60"/>
+      <c r="F92" s="60"/>
+      <c r="G92" s="60"/>
+      <c r="H92" s="60"/>
+      <c r="I92" s="60"/>
+      <c r="J92" s="60"/>
+      <c r="K92" s="60"/>
     </row>
     <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
@@ -8578,20 +8578,20 @@
       <c r="J96" s="29"/>
       <c r="K96" s="30"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="55" t="s">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B97" s="56"/>
-      <c r="C97" s="56"/>
-      <c r="D97" s="56"/>
-      <c r="E97" s="56"/>
-      <c r="F97" s="56"/>
-      <c r="G97" s="56"/>
-      <c r="H97" s="56"/>
-      <c r="I97" s="56"/>
-      <c r="J97" s="56"/>
-      <c r="K97" s="56"/>
+      <c r="B97" s="60"/>
+      <c r="C97" s="60"/>
+      <c r="D97" s="60"/>
+      <c r="E97" s="60"/>
+      <c r="F97" s="60"/>
+      <c r="G97" s="60"/>
+      <c r="H97" s="60"/>
+      <c r="I97" s="60"/>
+      <c r="J97" s="60"/>
+      <c r="K97" s="60"/>
     </row>
     <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
@@ -8637,15 +8637,21 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A61:K61"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A6:R6"/>
-    <mergeCell ref="A51:R51"/>
-    <mergeCell ref="A58:R58"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="A87:K87"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="R7:R21"/>
+    <mergeCell ref="R52:R57"/>
+    <mergeCell ref="R59:R60"/>
     <mergeCell ref="A92:K92"/>
     <mergeCell ref="A97:K97"/>
     <mergeCell ref="A4:A5"/>
@@ -8661,21 +8667,15 @@
     <mergeCell ref="A69:K69"/>
     <mergeCell ref="A72:K72"/>
     <mergeCell ref="A77:K77"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="A87:K87"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="R7:R21"/>
-    <mergeCell ref="R52:R57"/>
-    <mergeCell ref="R59:R60"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A61:K61"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A6:R6"/>
+    <mergeCell ref="A51:R51"/>
+    <mergeCell ref="A58:R58"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>